<commit_message>
Se agregó reporte General, se corrigió orden de las categorias de las graficas y se hicieron cambios en el archivo de puntajes
</commit_message>
<xml_diff>
--- a/Proyecto 1/Pruebas/Prueba1/Puntajes.xlsx
+++ b/Proyecto 1/Pruebas/Prueba1/Puntajes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192F7D5B-CF72-4E8D-A7B5-040F695212B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A416FC45-E2EE-4E57-9352-2D79CE413761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{428C83DC-4845-4F43-A285-B1AAA4F1AE4E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
   <si>
     <t>Proyecto A</t>
   </si>
@@ -199,12 +199,6 @@
     <t>No hay repitencia de identificador</t>
   </si>
   <si>
-    <t>Misma cantidad de paramteros que el metodo set_size</t>
-  </si>
-  <si>
-    <t>Misma cantidad de lineas que el metodo imprimir</t>
-  </si>
-  <si>
     <t>5 / 7</t>
   </si>
   <si>
@@ -253,12 +247,6 @@
     <t>fact_generator</t>
   </si>
   <si>
-    <t>Misma cantidad de parametros que el metodo fibonacci_generator</t>
-  </si>
-  <si>
-    <t>No tiene la misma cantidad de lineas que metodo torresDeHanoi</t>
-  </si>
-  <si>
     <t>// fibonacci iterativo</t>
   </si>
   <si>
@@ -269,6 +257,42 @@
   </si>
   <si>
     <t>0 / 10</t>
+  </si>
+  <si>
+    <t>Como no hizo match el id con ningun metodo se comparo numero de lineas y tampoco hizo match con ningun metodo</t>
+  </si>
+  <si>
+    <t>Como no hizo match el identificador y no hizo match el numero de lineas ya no se comparo el numero de parametros</t>
+  </si>
+  <si>
+    <t>Como no hizo match el identificador se comparo numero de lineas e hizo match con set_size</t>
+  </si>
+  <si>
+    <t>Como no hizo match el identificador pero si con las lineas de set_size se compara el numero de parametros el cual tambien hace match</t>
+  </si>
+  <si>
+    <t>No se repite el identificador</t>
+  </si>
+  <si>
+    <t>Se repite identificador</t>
+  </si>
+  <si>
+    <t>Se repite cantidad de parametros</t>
+  </si>
+  <si>
+    <t>No se repite la cantidad de lineas</t>
+  </si>
+  <si>
+    <t>Como no hace match el identificador se procede a comparar el numero de lineas; el numero de lineas hace match</t>
+  </si>
+  <si>
+    <t>Como no se hizo match con el identificador pero si el numero de lineas se comparo el numero de parametros que tambien hizo match</t>
+  </si>
+  <si>
+    <t>Como no hizo match el identificador se busco por cantidad de lineas; se hizo match con torresDeHanoi</t>
+  </si>
+  <si>
+    <t>Con no hizo match el identificador pero si el numero de lineas se procedio a compara el numero de parametros el cual no hace match</t>
   </si>
 </sst>
 </file>
@@ -357,18 +381,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2B342C-679D-4CCB-B18A-BD5C69CFD0AD}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +720,7 @@
     <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="88.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="138.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -727,7 +751,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>46</v>
@@ -756,10 +780,10 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="13"/>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -972,14 +996,14 @@
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="D25" s="9" t="s">
+      <c r="B25" s="13"/>
+      <c r="D25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="13"/>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -1036,14 +1060,14 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="D30" s="9" t="s">
+      <c r="B30" s="13"/>
+      <c r="D30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="10"/>
+      <c r="E30" s="13"/>
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -1100,14 +1124,14 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="D35" s="9" t="s">
+      <c r="B35" s="13"/>
+      <c r="D35" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="10"/>
+      <c r="E35" s="13"/>
       <c r="G35" t="s">
         <v>5</v>
       </c>
@@ -1134,16 +1158,16 @@
         <v>24</v>
       </c>
       <c r="B37" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E37" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1160,14 +1184,14 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="10"/>
+      <c r="B40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -1188,7 +1212,7 @@
         <v>0.3</v>
       </c>
       <c r="G42" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1199,7 +1223,7 @@
         <v>0.3</v>
       </c>
       <c r="G43" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -1271,14 +1295,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D46:E46"/>
@@ -1288,6 +1304,14 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1298,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EE6A5-91A5-4932-A55B-CBC652FE1ED4}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1308,7 +1332,7 @@
     <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="88.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1325,13 +1349,13 @@
         <v>47</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1339,13 +1363,13 @@
         <v>45</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1368,10 +1392,10 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="13"/>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -1392,7 +1416,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1411,7 +1435,7 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1457,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -1468,13 +1492,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -1485,13 +1509,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -1502,13 +1526,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -1521,7 +1545,7 @@
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="D19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -1534,7 +1558,7 @@
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -1548,8 +1572,8 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
@@ -1562,14 +1586,14 @@
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="D25" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="10"/>
+      <c r="A25" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="D25" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="13"/>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1612,7 @@
         <v>0.4</v>
       </c>
       <c r="G26" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1605,7 +1629,7 @@
         <v>0.3</v>
       </c>
       <c r="G27" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1622,18 +1646,18 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="D30" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="10"/>
+      <c r="A30" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="D30" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="13"/>
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -1652,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1669,7 +1693,7 @@
         <v>0.3</v>
       </c>
       <c r="G32" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1686,16 +1710,16 @@
         <v>0.3</v>
       </c>
       <c r="G33" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="D35" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="10"/>
+      <c r="D35" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="13"/>
       <c r="G35" t="s">
         <v>5</v>
       </c>
@@ -1720,10 +1744,10 @@
         <v>24</v>
       </c>
       <c r="E37" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1736,7 +1760,7 @@
         <v>0.3</v>
       </c>
       <c r="G38" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1778,7 +1802,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -1800,16 +1824,22 @@
       <c r="G48" s="6"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="13"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="13"/>
+      <c r="D49" s="10"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="D46:E46"/>
@@ -1819,12 +1849,6 @@
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregó comentario en file_2 de excel con hanoi_generator
</commit_message>
<xml_diff>
--- a/Proyecto 1/Pruebas/Prueba1/Puntajes.xlsx
+++ b/Proyecto 1/Pruebas/Prueba1/Puntajes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A416FC45-E2EE-4E57-9352-2D79CE413761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B9A0D5-9385-4B0B-923F-1C2067C0112E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{428C83DC-4845-4F43-A285-B1AAA4F1AE4E}"/>
+    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{428C83DC-4845-4F43-A285-B1AAA4F1AE4E}"/>
   </bookViews>
   <sheets>
     <sheet name="file_1.js" sheetId="1" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>No se repite la cantidad de lineas</t>
   </si>
   <si>
-    <t>Como no hace match el identificador se procede a comparar el numero de lineas; el numero de lineas hace match</t>
-  </si>
-  <si>
     <t>Como no se hizo match con el identificador pero si el numero de lineas se comparo el numero de parametros que tambien hizo match</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>Con no hizo match el identificador pero si el numero de lineas se procedio a compara el numero de parametros el cual no hace match</t>
+  </si>
+  <si>
+    <t>Como no hace match el identificador se procede a comparar el numero de lineas; el numero de lineas hace match con hanoi generator</t>
   </si>
 </sst>
 </file>
@@ -385,13 +385,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -710,7 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2B342C-679D-4CCB-B18A-BD5C69CFD0AD}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
@@ -761,29 +761,29 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="A5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="12"/>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -849,14 +849,14 @@
       <c r="F11" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="D14" s="11" t="s">
+      <c r="B14" s="13"/>
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="13"/>
       <c r="G14" t="s">
         <v>5</v>
       </c>
@@ -986,24 +986,24 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="D24" s="11" t="s">
+      <c r="B24" s="13"/>
+      <c r="D24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="D25" s="12" t="s">
+      <c r="B25" s="12"/>
+      <c r="D25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="12"/>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -1060,14 +1060,14 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="D30" s="12" t="s">
+      <c r="B30" s="12"/>
+      <c r="D30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="13"/>
+      <c r="E30" s="12"/>
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -1124,14 +1124,14 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="D35" s="12" t="s">
+      <c r="B35" s="12"/>
+      <c r="D35" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="12"/>
       <c r="G35" t="s">
         <v>5</v>
       </c>
@@ -1188,10 +1188,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="13"/>
+      <c r="B40" s="12"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -1230,14 +1230,14 @@
       <c r="F44" s="6"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="D46" s="11" t="s">
+      <c r="B46" s="13"/>
+      <c r="D46" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="11"/>
+      <c r="E46" s="13"/>
       <c r="F46" s="6"/>
       <c r="G46" t="s">
         <v>5</v>
@@ -1295,6 +1295,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D46:E46"/>
@@ -1304,14 +1312,6 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1322,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EE6A5-91A5-4932-A55B-CBC652FE1ED4}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="G24" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,29 +1373,29 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="A5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="12"/>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -1461,14 +1461,14 @@
       <c r="F11" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="D14" s="11" t="s">
+      <c r="B14" s="13"/>
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="13"/>
       <c r="G14" t="s">
         <v>5</v>
       </c>
@@ -1576,24 +1576,24 @@
       <c r="E22" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="D24" s="11" t="s">
+      <c r="B24" s="13"/>
+      <c r="D24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="D25" s="12" t="s">
+      <c r="B25" s="12"/>
+      <c r="D25" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="12"/>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -1650,14 +1650,14 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="D30" s="12" t="s">
+      <c r="B30" s="12"/>
+      <c r="D30" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="13"/>
+      <c r="E30" s="12"/>
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>0.3</v>
       </c>
       <c r="G32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1710,16 +1710,16 @@
         <v>0.3</v>
       </c>
       <c r="G33" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="12"/>
       <c r="G35" t="s">
         <v>5</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1760,7 +1760,7 @@
         <v>0.3</v>
       </c>
       <c r="G38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1787,14 +1787,14 @@
       <c r="F44" s="6"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="D46" s="11" t="s">
+      <c r="B46" s="13"/>
+      <c r="D46" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="11"/>
+      <c r="E46" s="13"/>
       <c r="F46" s="6"/>
       <c r="G46" t="s">
         <v>5</v>
@@ -1834,12 +1834,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="D46:E46"/>
@@ -1849,6 +1843,12 @@
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se corrigio archivo de puntajes
</commit_message>
<xml_diff>
--- a/Proyecto 1/Pruebas/Prueba1/Puntajes.xlsx
+++ b/Proyecto 1/Pruebas/Prueba1/Puntajes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B9A0D5-9385-4B0B-923F-1C2067C0112E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC4FB97-1CB5-44BC-81F7-2747FB07B206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{428C83DC-4845-4F43-A285-B1AAA4F1AE4E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{428C83DC-4845-4F43-A285-B1AAA4F1AE4E}"/>
   </bookViews>
   <sheets>
     <sheet name="file_1.js" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,6 @@
     <t>Apesar de que el /* del proyecto A esta identado si se cuenta a partir del /* ambos comentarios son exactamente iguales en identado, espacios, saltos de linea y texto</t>
   </si>
   <si>
-    <t>Puntaje General</t>
-  </si>
-  <si>
     <t>Variables Repetidas</t>
   </si>
   <si>
@@ -184,24 +181,15 @@
     <t>Comentarios repetidos</t>
   </si>
   <si>
-    <t>2 / 3</t>
-  </si>
-  <si>
     <t>0 / 2</t>
   </si>
   <si>
-    <t>8 / 14</t>
-  </si>
-  <si>
     <t>imprimir</t>
   </si>
   <si>
     <t>No hay repitencia de identificador</t>
   </si>
   <si>
-    <t>5 / 7</t>
-  </si>
-  <si>
     <t>La clase ejercicios numericos no tiene el mismo numero que complex exercises</t>
   </si>
   <si>
@@ -253,9 +241,6 @@
     <t>0 / 1</t>
   </si>
   <si>
-    <t>5 / 5</t>
-  </si>
-  <si>
     <t>0 / 10</t>
   </si>
   <si>
@@ -293,6 +278,21 @@
   </si>
   <si>
     <t>Como no hace match el identificador se procede a comparar el numero de lineas; el numero de lineas hace match con hanoi generator</t>
+  </si>
+  <si>
+    <t>1 / 5</t>
+  </si>
+  <si>
+    <t>3 / 7</t>
+  </si>
+  <si>
+    <t>4 / 14</t>
+  </si>
+  <si>
+    <t>Resumen</t>
+  </si>
+  <si>
+    <t>3 / 5</t>
   </si>
 </sst>
 </file>
@@ -385,13 +385,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2B342C-679D-4CCB-B18A-BD5C69CFD0AD}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,65 +725,62 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="7">
-        <f>(2/3*0.2)+(8/14*0.2)+(5/7*0.3)+(0/2*0.3)</f>
-        <v>0.46190476190476193</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="D5" s="13" t="s">
+      <c r="A5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="13"/>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -849,14 +846,14 @@
       <c r="F11" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="D14" s="13" t="s">
+      <c r="B14" s="11"/>
+      <c r="D14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="11"/>
       <c r="G14" t="s">
         <v>5</v>
       </c>
@@ -986,24 +983,24 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="D24" s="13" t="s">
+      <c r="B24" s="11"/>
+      <c r="D24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="13"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="D25" s="11" t="s">
+      <c r="B25" s="13"/>
+      <c r="D25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="13"/>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -1060,14 +1057,14 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="D30" s="11" t="s">
+      <c r="B30" s="13"/>
+      <c r="D30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="12"/>
+      <c r="E30" s="13"/>
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -1124,14 +1121,14 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="D35" s="11" t="s">
+      <c r="B35" s="13"/>
+      <c r="D35" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="12"/>
+      <c r="E35" s="13"/>
       <c r="G35" t="s">
         <v>5</v>
       </c>
@@ -1167,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1184,14 +1181,14 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="12"/>
+      <c r="A40" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -1201,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1212,7 +1209,7 @@
         <v>0.3</v>
       </c>
       <c r="G42" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1223,21 +1220,21 @@
         <v>0.3</v>
       </c>
       <c r="G43" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F44" s="6"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="D46" s="13" t="s">
+      <c r="B46" s="11"/>
+      <c r="D46" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="13"/>
+      <c r="E46" s="11"/>
       <c r="F46" s="6"/>
       <c r="G46" t="s">
         <v>5</v>
@@ -1295,14 +1292,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D46:E46"/>
@@ -1312,6 +1301,14 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1322,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EE6A5-91A5-4932-A55B-CBC652FE1ED4}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G24" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1337,65 +1334,62 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="7">
-        <f>1*0.3</f>
-        <v>0.3</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="D5" s="13" t="s">
+      <c r="A5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="13"/>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -1416,7 +1410,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1435,7 +1429,7 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1461,14 +1455,14 @@
       <c r="F11" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="D14" s="13" t="s">
+      <c r="B14" s="11"/>
+      <c r="D14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="11"/>
       <c r="G14" t="s">
         <v>5</v>
       </c>
@@ -1481,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -1492,13 +1486,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -1509,13 +1503,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -1526,13 +1520,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -1545,7 +1539,7 @@
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="D19" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -1558,7 +1552,7 @@
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="D20" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -1576,24 +1570,24 @@
       <c r="E22" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="D24" s="13" t="s">
+      <c r="B24" s="11"/>
+      <c r="D24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="13"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="D25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="12"/>
+      <c r="A25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="D25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="13"/>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -1612,7 +1606,7 @@
         <v>0.4</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1629,7 +1623,7 @@
         <v>0.3</v>
       </c>
       <c r="G27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1646,18 +1640,18 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="12"/>
-      <c r="D30" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="12"/>
+      <c r="A30" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="D30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="13"/>
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1693,7 +1687,7 @@
         <v>0.3</v>
       </c>
       <c r="G32" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1710,16 +1704,16 @@
         <v>0.3</v>
       </c>
       <c r="G33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="D35" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="12"/>
+      <c r="D35" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="13"/>
       <c r="G35" t="s">
         <v>5</v>
       </c>
@@ -1747,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1760,7 +1754,7 @@
         <v>0.3</v>
       </c>
       <c r="G38" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1787,14 +1781,14 @@
       <c r="F44" s="6"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="D46" s="13" t="s">
+      <c r="B46" s="11"/>
+      <c r="D46" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="13"/>
+      <c r="E46" s="11"/>
       <c r="F46" s="6"/>
       <c r="G46" t="s">
         <v>5</v>
@@ -1802,7 +1796,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -1834,6 +1828,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="D46:E46"/>
@@ -1843,12 +1843,6 @@
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se corrigio archivo de puntaje
</commit_message>
<xml_diff>
--- a/Proyecto 1/Pruebas/Prueba1/Puntajes.xlsx
+++ b/Proyecto 1/Pruebas/Prueba1/Puntajes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC4FB97-1CB5-44BC-81F7-2747FB07B206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{521BAD45-98FA-4904-BCE3-BAF82C9BB9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{428C83DC-4845-4F43-A285-B1AAA4F1AE4E}"/>
+    <workbookView xWindow="28680" yWindow="1515" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{428C83DC-4845-4F43-A285-B1AAA4F1AE4E}"/>
   </bookViews>
   <sheets>
     <sheet name="file_1.js" sheetId="1" r:id="rId1"/>
@@ -256,9 +256,6 @@
     <t>Como no hizo match el identificador pero si con las lineas de set_size se compara el numero de parametros el cual tambien hace match</t>
   </si>
   <si>
-    <t>No se repite el identificador</t>
-  </si>
-  <si>
     <t>Se repite identificador</t>
   </si>
   <si>
@@ -268,18 +265,6 @@
     <t>No se repite la cantidad de lineas</t>
   </si>
   <si>
-    <t>Como no se hizo match con el identificador pero si el numero de lineas se comparo el numero de parametros que tambien hizo match</t>
-  </si>
-  <si>
-    <t>Como no hizo match el identificador se busco por cantidad de lineas; se hizo match con torresDeHanoi</t>
-  </si>
-  <si>
-    <t>Con no hizo match el identificador pero si el numero de lineas se procedio a compara el numero de parametros el cual no hace match</t>
-  </si>
-  <si>
-    <t>Como no hace match el identificador se procede a comparar el numero de lineas; el numero de lineas hace match con hanoi generator</t>
-  </si>
-  <si>
     <t>1 / 5</t>
   </si>
   <si>
@@ -292,7 +277,22 @@
     <t>Resumen</t>
   </si>
   <si>
-    <t>3 / 5</t>
+    <t>No se repite ningun identificador</t>
+  </si>
+  <si>
+    <t>El numero de parametros entre torresDeHanoi no hace match con fibonacci_generator; por el contrario hanoi_generator hace match con torresDeHanoi</t>
+  </si>
+  <si>
+    <t>El numero de lineas de torresDeHanoi hace match con fibonacci_generator; por el contrario el numero de lineas de hanoi_generator hace match con torresDeHanoi</t>
+  </si>
+  <si>
+    <t>No hizo match con ningun metodo</t>
+  </si>
+  <si>
+    <t>Como no hizo match en lineas no se comparan parametros</t>
+  </si>
+  <si>
+    <t>2 / 5</t>
   </si>
 </sst>
 </file>
@@ -385,13 +385,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -725,7 +725,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -734,13 +734,13 @@
         <v>46</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -748,7 +748,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>45</v>
@@ -758,29 +758,29 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="A5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="12"/>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -846,14 +846,14 @@
       <c r="F11" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="D14" s="11" t="s">
+      <c r="B14" s="13"/>
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="13"/>
       <c r="G14" t="s">
         <v>5</v>
       </c>
@@ -983,24 +983,24 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="D24" s="11" t="s">
+      <c r="B24" s="13"/>
+      <c r="D24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="D25" s="12" t="s">
+      <c r="B25" s="12"/>
+      <c r="D25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="12"/>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -1057,14 +1057,14 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="D30" s="12" t="s">
+      <c r="B30" s="12"/>
+      <c r="D30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="13"/>
+      <c r="E30" s="12"/>
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -1121,14 +1121,14 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="D35" s="12" t="s">
+      <c r="B35" s="12"/>
+      <c r="D35" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="12"/>
       <c r="G35" t="s">
         <v>5</v>
       </c>
@@ -1185,10 +1185,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="13"/>
+      <c r="B40" s="12"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -1227,14 +1227,14 @@
       <c r="F44" s="6"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="D46" s="11" t="s">
+      <c r="B46" s="13"/>
+      <c r="D46" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="11"/>
+      <c r="E46" s="13"/>
       <c r="F46" s="6"/>
       <c r="G46" t="s">
         <v>5</v>
@@ -1292,6 +1292,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D46:E46"/>
@@ -1301,14 +1309,6 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1319,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EE6A5-91A5-4932-A55B-CBC652FE1ED4}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1334,7 +1334,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -1367,29 +1367,29 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="A5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="12"/>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -1455,14 +1455,14 @@
       <c r="F11" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="D14" s="11" t="s">
+      <c r="B14" s="13"/>
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="13"/>
       <c r="G14" t="s">
         <v>5</v>
       </c>
@@ -1570,24 +1570,24 @@
       <c r="E22" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="D24" s="11" t="s">
+      <c r="B24" s="13"/>
+      <c r="D24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="D25" s="12" t="s">
+      <c r="B25" s="12"/>
+      <c r="D25" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="12"/>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>0.4</v>
       </c>
       <c r="G26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1623,7 +1623,7 @@
         <v>0.3</v>
       </c>
       <c r="G27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1640,18 +1640,18 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="D30" s="12" t="s">
+      <c r="B30" s="12"/>
+      <c r="D30" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="13"/>
+      <c r="E30" s="12"/>
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1678,7 +1678,7 @@
         <v>24</v>
       </c>
       <c r="B32" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>24</v>
@@ -1687,7 +1687,7 @@
         <v>0.3</v>
       </c>
       <c r="G32" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1704,16 +1704,16 @@
         <v>0.3</v>
       </c>
       <c r="G33" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="12"/>
       <c r="G35" t="s">
         <v>5</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1751,10 +1751,10 @@
         <v>25</v>
       </c>
       <c r="E38" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1781,14 +1781,14 @@
       <c r="F44" s="6"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="D46" s="11" t="s">
+      <c r="B46" s="13"/>
+      <c r="D46" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="11"/>
+      <c r="E46" s="13"/>
       <c r="F46" s="6"/>
       <c r="G46" t="s">
         <v>5</v>
@@ -1828,12 +1828,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="D46:E46"/>
@@ -1843,6 +1837,12 @@
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>